<commit_message>
+Unicorn name generator • Using Orchestrator Queue, add 10 Names and Months to the queue • Using RE Framework build a solution to extract the Unicorn Name and save it into Excel. URL: http://www.rpasamples.com/unicornname
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rencita.Monteiro\Documents\UiPath\Assignment_10\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB45A0C-C637-46FF-9853-CE05B88D51D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,10 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>InputDetails</t>
+  </si>
+  <si>
+    <t>RPATraining</t>
   </si>
 </sst>
 </file>
@@ -212,10 +215,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,9 +242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +282,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +388,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,12 +544,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,17 +597,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1619,16 +1624,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1670,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1795,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2787,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
+ Completed with annotations and changed activity names
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rencita.Monteiro\Documents\UiPath\Assignment_10\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7dc8928f65293786/Documents/UiPath/Rencita_Day_3/Rencita_Day_10/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB45A0C-C637-46FF-9853-CE05B88D51D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7EB45A0C-C637-46FF-9853-CE05B88D51D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F45D4216-A52A-4A80-9533-82E3D236A8B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -163,13 +163,49 @@
   </si>
   <si>
     <t>RPATraining</t>
+  </si>
+  <si>
+    <t>BrowserURL</t>
+  </si>
+  <si>
+    <t>https://www.rpasamples.com/unicornname</t>
+  </si>
+  <si>
+    <t>Input File path</t>
+  </si>
+  <si>
+    <t>Data\Input\input_Unicorn_names.xlsx</t>
+  </si>
+  <si>
+    <t>InputSheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue folder name </t>
+  </si>
+  <si>
+    <t>Queue name</t>
+  </si>
+  <si>
+    <t>Data/Output/UnicornName.xlsx</t>
+  </si>
+  <si>
+    <t>Output file path</t>
+  </si>
+  <si>
+    <t>UnicornName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output sheet name </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +229,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,10 +253,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -224,8 +267,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -242,9 +287,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,7 +327,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -388,7 +433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -540,16 +585,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -597,7 +642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -609,7 +654,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -620,13 +665,62 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1615,8 +1709,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{0B63B7E7-35B3-4FEE-A082-4FAE86170879}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1624,16 +1721,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1767,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1681,7 +1778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1795,7 +1892,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2789,12 +2886,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>